<commit_message>
testes com Recipe Exception2
</commit_message>
<xml_diff>
--- a/Plano de testes.xlsx
+++ b/Plano de testes.xlsx
@@ -9,6 +9,7 @@
   </bookViews>
   <sheets>
     <sheet name="Classes de Equivalência" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Obs." sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="123">
   <si>
     <t xml:space="preserve">Classe</t>
   </si>
@@ -375,6 +376,21 @@
   </si>
   <si>
     <t xml:space="preserve">3 e 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se não fizer Teste contínuo/Regressão, o que garante qualidade minima de coisa que funciona?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se não fizer Refatoração, cresce a complexidade</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se não fazer integração contínua, fica caótico deixar disponibilidade</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Testes, trazem provas que o software não funciona</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Criar Classes de equivalencia: das infinitas possibilidade usa o limite, limite+1 e o limite-1</t>
   </si>
 </sst>
 </file>
@@ -505,8 +521,8 @@
   </sheetPr>
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1:H33"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -516,7 +532,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="29.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="48.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="34.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="32.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="32.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="21.44"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="11.52"/>
   </cols>
@@ -1166,4 +1182,57 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="69.79"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>122</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>